<commit_message>
Data for richter correction
</commit_message>
<xml_diff>
--- a/data/richter_parameters.xlsx
+++ b/data/richter_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghnfa\OneDrive\Desktop\Research Project\Ilmenau\R files\Data Preparation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\ghnfarid\Projects\meteo-interp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EEEDD0-7DF5-415A-B0FF-12BCFB752CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F97DCED-1A1C-4D8A-A133-B8A2C657422B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="3435" windowWidth="21600" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>maximum changes</t>
-  </si>
-  <si>
     <t>Summer_month_Start</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>T_Mix</t>
+  </si>
+  <si>
+    <t>maximum_changes</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,43 +419,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>